<commit_message>
- Actualización de templates de los paises para agregar el Victoria 162/163 - Actualizacion de templates de Dominica - Actualizacion de templates de virus - Agregar template Lineas Basales para Dominica y Colombia - Agregar FLUID para Dominica y Colombia - Agregar todos los reportes para Dominica
</commit_message>
<xml_diff>
--- a/Template/Export/Sari_Cases_18.xlsx
+++ b/Template/Export/Sari_Cases_18.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="229">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="229" uniqueCount="229">
   <si>
     <t>ID</t>
   </si>
@@ -781,7 +781,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="16">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -790,7 +790,6 @@
     <xf numFmtId="1" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="164" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="167" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1114,11 +1113,11 @@
     <col min="2" max="2" width="55.85546875" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="13.7109375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="17.85546875" style="2" customWidth="1"/>
-    <col min="6" max="6" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="17.5703125" style="2" customWidth="1"/>
     <col min="7" max="7" width="16.85546875" customWidth="1"/>
-    <col min="8" max="8" width="18.7109375" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="19.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="32.42578125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="16.42578125" customWidth="1"/>
+    <col min="9" max="9" width="15.85546875" style="9" customWidth="1"/>
+    <col min="10" max="10" width="20.28515625" customWidth="1"/>
     <col min="11" max="11" width="27.28515625" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="32.42578125" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="27.28515625" bestFit="1" customWidth="1"/>
@@ -1130,27 +1129,31 @@
     <col min="22" max="22" width="25.28515625" customWidth="1"/>
     <col min="23" max="23" width="23.42578125" customWidth="1"/>
     <col min="24" max="24" width="21.7109375" customWidth="1"/>
-    <col min="25" max="25" width="20.85546875" customWidth="1"/>
-    <col min="26" max="26" width="21.28515625" customWidth="1"/>
-    <col min="27" max="27" width="20.42578125" customWidth="1"/>
+    <col min="25" max="25" width="8.28515625" customWidth="1"/>
+    <col min="26" max="26" width="11.85546875" customWidth="1"/>
+    <col min="27" max="27" width="6.7109375" customWidth="1"/>
     <col min="28" max="28" width="17.42578125" customWidth="1"/>
-    <col min="29" max="29" width="33.28515625" customWidth="1"/>
+    <col min="29" max="29" width="13.28515625" customWidth="1"/>
     <col min="30" max="30" width="6.7109375" bestFit="1" customWidth="1"/>
     <col min="31" max="31" width="8.140625" bestFit="1" customWidth="1"/>
     <col min="32" max="32" width="9.7109375" bestFit="1" customWidth="1"/>
     <col min="33" max="38" width="9.7109375" customWidth="1"/>
     <col min="39" max="39" width="30.5703125" bestFit="1" customWidth="1"/>
     <col min="40" max="40" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="41" max="46" width="9.7109375" customWidth="1"/>
+    <col min="41" max="41" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="27.5703125" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="19.85546875" customWidth="1"/>
+    <col min="44" max="44" width="13.85546875" customWidth="1"/>
+    <col min="45" max="46" width="9.7109375" customWidth="1"/>
     <col min="47" max="47" width="21.42578125" bestFit="1" customWidth="1"/>
-    <col min="48" max="48" width="27.42578125" bestFit="1" customWidth="1"/>
+    <col min="48" max="48" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="49" max="49" width="26.85546875" bestFit="1" customWidth="1"/>
     <col min="53" max="53" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="54" max="54" width="17.5703125" bestFit="1" customWidth="1"/>
     <col min="55" max="55" width="15" style="2" bestFit="1" customWidth="1"/>
     <col min="56" max="56" width="17.85546875" style="2" bestFit="1" customWidth="1"/>
     <col min="57" max="57" width="18.42578125" bestFit="1" customWidth="1"/>
-    <col min="58" max="58" width="16.42578125" bestFit="1" customWidth="1"/>
+    <col min="58" max="58" width="16.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="59" max="59" width="16.7109375" bestFit="1" customWidth="1"/>
     <col min="61" max="61" width="14.5703125" style="2" customWidth="1"/>
     <col min="62" max="62" width="14.28515625" bestFit="1" customWidth="1"/>
@@ -1184,21 +1187,21 @@
     <col min="127" max="127" width="10.28515625" bestFit="1" customWidth="1"/>
     <col min="128" max="128" width="21" style="2" bestFit="1" customWidth="1"/>
     <col min="129" max="130" width="21" style="2" customWidth="1"/>
-    <col min="131" max="131" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="131" max="131" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="132" max="132" width="9" bestFit="1" customWidth="1"/>
-    <col min="133" max="133" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
-    <col min="135" max="135" width="11.42578125" style="8" customWidth="1"/>
+    <col min="133" max="133" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="135" max="135" width="12.5703125" style="2" customWidth="1"/>
     <col min="137" max="137" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="138" max="138" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="140" max="140" width="13" style="2" bestFit="1" customWidth="1"/>
     <col min="141" max="141" width="29.5703125" bestFit="1" customWidth="1"/>
-    <col min="142" max="142" width="19.28515625" style="8" bestFit="1" customWidth="1"/>
+    <col min="142" max="142" width="19.28515625" style="2" bestFit="1" customWidth="1"/>
     <col min="143" max="143" width="21" bestFit="1" customWidth="1"/>
     <col min="145" max="145" width="13.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="146" max="146" width="37.85546875" customWidth="1"/>
-    <col min="147" max="147" width="22.42578125" style="8" bestFit="1" customWidth="1"/>
+    <col min="147" max="147" width="22.42578125" style="2" bestFit="1" customWidth="1"/>
     <col min="149" max="149" width="20.140625" bestFit="1" customWidth="1"/>
-    <col min="150" max="150" width="18.7109375" style="8" bestFit="1" customWidth="1"/>
+    <col min="150" max="150" width="18.7109375" style="2" bestFit="1" customWidth="1"/>
     <col min="151" max="151" width="12.42578125" bestFit="1" customWidth="1"/>
     <col min="152" max="152" width="11.42578125" bestFit="1" customWidth="1"/>
     <col min="153" max="153" width="14.42578125" bestFit="1" customWidth="1"/>
@@ -1229,6 +1232,7 @@
     <col min="178" max="178" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="179" max="179" width="21.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="180" max="180" width="21.28515625" style="2" bestFit="1" customWidth="1"/>
+    <col min="181" max="181" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="183" max="183" width="16.85546875" bestFit="1" customWidth="1"/>
     <col min="184" max="184" width="18" bestFit="1" customWidth="1"/>
     <col min="185" max="185" width="16.140625" bestFit="1" customWidth="1"/>
@@ -1243,7 +1247,7 @@
     <col min="196" max="196" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="197" max="197" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="198" max="198" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="199" max="199" width="19.28515625" customWidth="1"/>
+    <col min="199" max="199" width="24.5703125" bestFit="1" customWidth="1"/>
     <col min="200" max="200" width="24.140625" bestFit="1" customWidth="1"/>
     <col min="201" max="201" width="21.140625" style="2" bestFit="1" customWidth="1"/>
     <col min="202" max="202" width="21.28515625" style="2" bestFit="1" customWidth="1"/>
@@ -1260,15 +1264,15 @@
     <col min="218" max="218" width="16.140625" bestFit="1" customWidth="1"/>
     <col min="219" max="219" width="13.85546875" bestFit="1" customWidth="1"/>
     <col min="220" max="220" width="20.42578125" bestFit="1" customWidth="1"/>
-    <col min="221" max="221" width="19.5703125" customWidth="1"/>
-    <col min="222" max="222" width="24.140625" bestFit="1" customWidth="1"/>
+    <col min="221" max="221" width="24.5703125" bestFit="1" customWidth="1"/>
+    <col min="222" max="222" width="21.5703125" bestFit="1" customWidth="1"/>
     <col min="223" max="223" width="19.42578125" style="2" bestFit="1" customWidth="1"/>
-    <col min="224" max="224" width="21.28515625" style="2" bestFit="1" customWidth="1"/>
-    <col min="225" max="225" width="23" bestFit="1" customWidth="1"/>
-    <col min="226" max="226" width="19.7109375" bestFit="1" customWidth="1"/>
-    <col min="227" max="227" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="228" max="228" width="18" bestFit="1" customWidth="1"/>
-    <col min="229" max="229" width="16.140625" bestFit="1" customWidth="1"/>
+    <col min="224" max="224" width="18.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="225" max="225" width="13.85546875" bestFit="1" customWidth="1"/>
+    <col min="226" max="226" width="15" bestFit="1" customWidth="1"/>
+    <col min="227" max="227" width="14.140625" bestFit="1" customWidth="1"/>
+    <col min="228" max="228" width="17" bestFit="1" customWidth="1"/>
+    <col min="229" max="229" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:229" x14ac:dyDescent="0.25">
@@ -1296,7 +1300,7 @@
       <c r="H1" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="9" t="s">
+      <c r="I1" s="8" t="s">
         <v>8</v>
       </c>
       <c r="J1" s="3" t="s">
@@ -1311,7 +1315,7 @@
       <c r="M1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="N1" s="11" t="s">
+      <c r="N1" s="10" t="s">
         <v>129</v>
       </c>
       <c r="O1" s="5" t="s">
@@ -1326,19 +1330,19 @@
       <c r="R1" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="S1" s="12" t="s">
+      <c r="S1" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="T1" s="12" t="s">
+      <c r="T1" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="U1" s="12" t="s">
+      <c r="U1" s="11" t="s">
         <v>19</v>
       </c>
-      <c r="V1" s="12" t="s">
+      <c r="V1" s="11" t="s">
         <v>20</v>
       </c>
-      <c r="W1" s="12" t="s">
+      <c r="W1" s="11" t="s">
         <v>21</v>
       </c>
       <c r="X1" s="3" t="s">
@@ -1353,7 +1357,7 @@
       <c r="AA1" s="3" t="s">
         <v>133</v>
       </c>
-      <c r="AB1" s="12" t="s">
+      <c r="AB1" s="11" t="s">
         <v>22</v>
       </c>
       <c r="AC1" s="3" t="s">
@@ -1368,55 +1372,55 @@
       <c r="AF1" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="AG1" s="12" t="s">
+      <c r="AG1" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="AH1" s="12" t="s">
+      <c r="AH1" s="11" t="s">
         <v>28</v>
       </c>
-      <c r="AI1" s="12" t="s">
+      <c r="AI1" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="AJ1" s="12" t="s">
+      <c r="AJ1" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="AK1" s="12" t="s">
+      <c r="AK1" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="AL1" s="12" t="s">
+      <c r="AL1" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="AM1" s="12" t="s">
+      <c r="AM1" s="11" t="s">
         <v>33</v>
       </c>
-      <c r="AN1" s="12" t="s">
+      <c r="AN1" s="11" t="s">
         <v>34</v>
       </c>
-      <c r="AO1" s="12" t="s">
+      <c r="AO1" s="11" t="s">
         <v>35</v>
       </c>
-      <c r="AP1" s="12" t="s">
+      <c r="AP1" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="AQ1" s="12" t="s">
+      <c r="AQ1" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="AR1" s="12" t="s">
+      <c r="AR1" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="AS1" s="12" t="s">
+      <c r="AS1" s="11" t="s">
         <v>39</v>
       </c>
-      <c r="AT1" s="12" t="s">
+      <c r="AT1" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="AU1" s="12" t="s">
+      <c r="AU1" s="11" t="s">
         <v>41</v>
       </c>
-      <c r="AV1" s="12" t="s">
+      <c r="AV1" s="11" t="s">
         <v>42</v>
       </c>
-      <c r="AW1" s="12" t="s">
+      <c r="AW1" s="11" t="s">
         <v>43</v>
       </c>
       <c r="AX1" s="3" t="s">
@@ -1434,7 +1438,7 @@
       <c r="BB1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="BC1" s="11" t="s">
+      <c r="BC1" s="10" t="s">
         <v>135</v>
       </c>
       <c r="BD1" s="4" t="s">
@@ -1443,7 +1447,7 @@
       <c r="BE1" s="3" t="s">
         <v>137</v>
       </c>
-      <c r="BF1" s="11" t="s">
+      <c r="BF1" s="10" t="s">
         <v>138</v>
       </c>
       <c r="BG1" s="3" t="s">
@@ -1494,13 +1498,13 @@
       <c r="BV1" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="BW1" s="12" t="s">
+      <c r="BW1" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="BX1" s="12" t="s">
+      <c r="BX1" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="BY1" s="12" t="s">
+      <c r="BY1" s="11" t="s">
         <v>63</v>
       </c>
       <c r="BZ1" s="3" t="s">
@@ -1542,7 +1546,7 @@
       <c r="CL1" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="CM1" s="12" t="s">
+      <c r="CM1" s="11" t="s">
         <v>76</v>
       </c>
       <c r="CN1" s="3" t="s">
@@ -1551,94 +1555,94 @@
       <c r="CO1" s="3" t="s">
         <v>143</v>
       </c>
-      <c r="CP1" s="12" t="s">
+      <c r="CP1" s="11" t="s">
         <v>78</v>
       </c>
-      <c r="CQ1" s="12" t="s">
+      <c r="CQ1" s="11" t="s">
         <v>144</v>
       </c>
-      <c r="CR1" s="12" t="s">
+      <c r="CR1" s="11" t="s">
         <v>145</v>
       </c>
-      <c r="CS1" s="12" t="s">
+      <c r="CS1" s="11" t="s">
         <v>79</v>
       </c>
-      <c r="CT1" s="12" t="s">
+      <c r="CT1" s="11" t="s">
         <v>80</v>
       </c>
-      <c r="CU1" s="12" t="s">
+      <c r="CU1" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="CV1" s="12" t="s">
+      <c r="CV1" s="11" t="s">
         <v>82</v>
       </c>
-      <c r="CW1" s="12" t="s">
+      <c r="CW1" s="11" t="s">
         <v>83</v>
       </c>
-      <c r="CX1" s="12" t="s">
+      <c r="CX1" s="11" t="s">
         <v>84</v>
       </c>
-      <c r="CY1" s="12" t="s">
+      <c r="CY1" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="CZ1" s="12" t="s">
+      <c r="CZ1" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="DA1" s="12" t="s">
+      <c r="DA1" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="DB1" s="12" t="s">
+      <c r="DB1" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="DC1" s="12" t="s">
+      <c r="DC1" s="11" t="s">
         <v>146</v>
       </c>
-      <c r="DD1" s="12" t="s">
+      <c r="DD1" s="11" t="s">
         <v>147</v>
       </c>
-      <c r="DE1" s="12" t="s">
+      <c r="DE1" s="11" t="s">
         <v>89</v>
       </c>
-      <c r="DF1" s="12" t="s">
+      <c r="DF1" s="11" t="s">
         <v>90</v>
       </c>
-      <c r="DG1" s="12" t="s">
+      <c r="DG1" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="DH1" s="12" t="s">
+      <c r="DH1" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="DI1" s="12" t="s">
+      <c r="DI1" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="DJ1" s="12" t="s">
+      <c r="DJ1" s="11" t="s">
         <v>148</v>
       </c>
-      <c r="DK1" s="12" t="s">
+      <c r="DK1" s="11" t="s">
         <v>149</v>
       </c>
-      <c r="DL1" s="12" t="s">
+      <c r="DL1" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="DM1" s="12" t="s">
+      <c r="DM1" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="DN1" s="12" t="s">
+      <c r="DN1" s="11" t="s">
         <v>96</v>
       </c>
-      <c r="DO1" s="12" t="s">
+      <c r="DO1" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="DP1" s="12" t="s">
+      <c r="DP1" s="11" t="s">
         <v>98</v>
       </c>
-      <c r="DQ1" s="12" t="s">
+      <c r="DQ1" s="11" t="s">
         <v>99</v>
       </c>
-      <c r="DR1" s="12" t="s">
+      <c r="DR1" s="11" t="s">
         <v>100</v>
       </c>
-      <c r="DS1" s="12" t="s">
+      <c r="DS1" s="11" t="s">
         <v>101</v>
       </c>
       <c r="DT1" s="3" t="s">
@@ -1656,10 +1660,10 @@
       <c r="DX1" s="4" t="s">
         <v>105</v>
       </c>
-      <c r="DY1" s="12" t="s">
+      <c r="DY1" s="11" t="s">
         <v>106</v>
       </c>
-      <c r="DZ1" s="14" t="s">
+      <c r="DZ1" s="13" t="s">
         <v>107</v>
       </c>
       <c r="EA1" s="7" t="s">
@@ -1725,40 +1729,40 @@
       <c r="EU1" s="3" t="s">
         <v>128</v>
       </c>
-      <c r="EV1" s="13" t="s">
+      <c r="EV1" s="12" t="s">
         <v>217</v>
       </c>
-      <c r="EW1" s="13" t="s">
+      <c r="EW1" s="12" t="s">
         <v>218</v>
       </c>
-      <c r="EX1" s="13" t="s">
+      <c r="EX1" s="12" t="s">
         <v>219</v>
       </c>
-      <c r="EY1" s="13" t="s">
+      <c r="EY1" s="12" t="s">
         <v>220</v>
       </c>
-      <c r="EZ1" s="15" t="s">
+      <c r="EZ1" s="14" t="s">
         <v>221</v>
       </c>
-      <c r="FA1" s="15" t="s">
+      <c r="FA1" s="14" t="s">
         <v>222</v>
       </c>
-      <c r="FB1" s="15" t="s">
+      <c r="FB1" s="14" t="s">
         <v>223</v>
       </c>
-      <c r="FC1" s="15" t="s">
+      <c r="FC1" s="14" t="s">
         <v>224</v>
       </c>
-      <c r="FD1" s="13" t="s">
+      <c r="FD1" s="12" t="s">
         <v>225</v>
       </c>
-      <c r="FE1" s="13" t="s">
+      <c r="FE1" s="12" t="s">
         <v>226</v>
       </c>
-      <c r="FF1" s="13" t="s">
+      <c r="FF1" s="12" t="s">
         <v>227</v>
       </c>
-      <c r="FG1" s="13" t="s">
+      <c r="FG1" s="12" t="s">
         <v>228</v>
       </c>
       <c r="FH1" s="3" t="s">
@@ -1961,42 +1965,27 @@
       </c>
     </row>
     <row r="2" spans="1:229" x14ac:dyDescent="0.25">
-      <c r="BD2"/>
       <c r="DZ2"/>
     </row>
     <row r="3" spans="1:229" x14ac:dyDescent="0.25">
-      <c r="BD3"/>
       <c r="DZ3"/>
     </row>
     <row r="4" spans="1:229" x14ac:dyDescent="0.25">
-      <c r="BC4" s="11" t="s">
-        <v>135</v>
-      </c>
-      <c r="BD4" s="4" t="s">
-        <v>136</v>
-      </c>
-      <c r="BE4" s="3" t="s">
-        <v>137</v>
-      </c>
-      <c r="BF4" s="11" t="s">
-        <v>138</v>
-      </c>
-      <c r="BG4" s="3" t="s">
-        <v>139</v>
-      </c>
+      <c r="BC4" s="10"/>
+      <c r="BD4" s="4"/>
+      <c r="BE4" s="3"/>
+      <c r="BF4" s="4"/>
+      <c r="BG4" s="3"/>
       <c r="DZ4"/>
     </row>
     <row r="5" spans="1:229" x14ac:dyDescent="0.25">
-      <c r="BD5"/>
       <c r="DZ5"/>
     </row>
     <row r="6" spans="1:229" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="BD6"/>
       <c r="DZ6"/>
       <c r="FK6" s="1"/>
     </row>
     <row r="7" spans="1:229" x14ac:dyDescent="0.25">
-      <c r="BD7"/>
       <c r="DZ7"/>
       <c r="FL7"/>
       <c r="FM7"/>
@@ -2012,2795 +2001,2097 @@
       <c r="HP7"/>
     </row>
     <row r="8" spans="1:229" x14ac:dyDescent="0.25">
-      <c r="BD8"/>
       <c r="DZ8"/>
     </row>
     <row r="9" spans="1:229" x14ac:dyDescent="0.25">
-      <c r="BD9"/>
       <c r="DZ9"/>
     </row>
     <row r="10" spans="1:229" x14ac:dyDescent="0.25">
-      <c r="BD10"/>
       <c r="DZ10"/>
     </row>
     <row r="11" spans="1:229" x14ac:dyDescent="0.25">
-      <c r="BD11"/>
       <c r="DZ11"/>
     </row>
     <row r="12" spans="1:229" x14ac:dyDescent="0.25">
-      <c r="BD12"/>
       <c r="DZ12"/>
     </row>
     <row r="13" spans="1:229" x14ac:dyDescent="0.25">
-      <c r="BD13"/>
       <c r="DZ13"/>
     </row>
     <row r="14" spans="1:229" x14ac:dyDescent="0.25">
-      <c r="BD14"/>
       <c r="DZ14"/>
     </row>
     <row r="15" spans="1:229" x14ac:dyDescent="0.25">
-      <c r="BD15"/>
       <c r="DZ15"/>
     </row>
     <row r="16" spans="1:229" x14ac:dyDescent="0.25">
-      <c r="BD16"/>
       <c r="DZ16"/>
     </row>
-    <row r="17" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD17"/>
+    <row r="17" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ17"/>
     </row>
-    <row r="18" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD18"/>
+    <row r="18" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ18"/>
     </row>
-    <row r="19" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD19"/>
+    <row r="19" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ19"/>
     </row>
-    <row r="20" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD20"/>
+    <row r="20" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ20"/>
     </row>
-    <row r="21" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD21"/>
+    <row r="21" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ21"/>
     </row>
-    <row r="22" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD22"/>
+    <row r="22" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ22"/>
     </row>
-    <row r="23" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD23"/>
+    <row r="23" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ23"/>
     </row>
-    <row r="24" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD24"/>
+    <row r="24" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ24"/>
     </row>
-    <row r="25" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD25"/>
+    <row r="25" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ25"/>
     </row>
-    <row r="26" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD26"/>
+    <row r="26" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ26"/>
     </row>
-    <row r="27" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD27"/>
+    <row r="27" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ27"/>
     </row>
-    <row r="28" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD28"/>
+    <row r="28" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ28"/>
     </row>
-    <row r="29" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD29"/>
+    <row r="29" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ29"/>
     </row>
-    <row r="30" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD30"/>
+    <row r="30" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ30"/>
     </row>
-    <row r="31" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD31"/>
+    <row r="31" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ31"/>
     </row>
-    <row r="32" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD32"/>
+    <row r="32" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ32"/>
     </row>
-    <row r="33" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD33"/>
+    <row r="33" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ33"/>
     </row>
-    <row r="34" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD34"/>
+    <row r="34" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ34"/>
     </row>
-    <row r="35" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD35"/>
+    <row r="35" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ35"/>
     </row>
-    <row r="36" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD36"/>
+    <row r="36" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ36"/>
     </row>
-    <row r="37" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD37"/>
+    <row r="37" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ37"/>
     </row>
-    <row r="38" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD38"/>
+    <row r="38" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ38"/>
     </row>
-    <row r="39" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD39"/>
+    <row r="39" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ39"/>
     </row>
-    <row r="40" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD40"/>
+    <row r="40" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ40"/>
     </row>
-    <row r="41" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD41"/>
+    <row r="41" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ41"/>
     </row>
-    <row r="42" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD42"/>
+    <row r="42" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ42"/>
     </row>
-    <row r="43" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD43"/>
+    <row r="43" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ43"/>
     </row>
-    <row r="44" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD44"/>
+    <row r="44" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ44"/>
     </row>
-    <row r="45" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD45"/>
+    <row r="45" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ45"/>
     </row>
-    <row r="46" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD46"/>
+    <row r="46" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ46"/>
     </row>
-    <row r="47" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD47"/>
+    <row r="47" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ47"/>
     </row>
-    <row r="48" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD48"/>
+    <row r="48" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ48"/>
     </row>
-    <row r="49" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD49"/>
+    <row r="49" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ49"/>
     </row>
-    <row r="50" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD50"/>
+    <row r="50" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ50"/>
     </row>
-    <row r="51" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD51"/>
+    <row r="51" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ51"/>
     </row>
-    <row r="52" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD52"/>
+    <row r="52" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ52"/>
     </row>
-    <row r="53" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD53"/>
+    <row r="53" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ53"/>
     </row>
-    <row r="54" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD54"/>
+    <row r="54" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ54"/>
     </row>
-    <row r="55" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD55"/>
+    <row r="55" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ55"/>
     </row>
-    <row r="56" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD56"/>
+    <row r="56" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ56"/>
     </row>
-    <row r="57" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD57"/>
+    <row r="57" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ57"/>
     </row>
-    <row r="58" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD58"/>
+    <row r="58" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ58"/>
     </row>
-    <row r="59" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD59"/>
+    <row r="59" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ59"/>
     </row>
-    <row r="60" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD60"/>
+    <row r="60" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ60"/>
     </row>
-    <row r="61" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD61"/>
+    <row r="61" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ61"/>
     </row>
-    <row r="62" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD62"/>
+    <row r="62" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ62"/>
     </row>
-    <row r="63" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD63"/>
+    <row r="63" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ63"/>
     </row>
-    <row r="64" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD64"/>
+    <row r="64" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ64"/>
     </row>
-    <row r="65" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD65"/>
+    <row r="65" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ65"/>
     </row>
-    <row r="66" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD66"/>
+    <row r="66" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ66"/>
     </row>
-    <row r="67" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD67"/>
+    <row r="67" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ67"/>
     </row>
-    <row r="68" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD68"/>
+    <row r="68" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ68"/>
     </row>
-    <row r="69" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD69"/>
+    <row r="69" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ69"/>
     </row>
-    <row r="70" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD70"/>
+    <row r="70" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ70"/>
     </row>
-    <row r="71" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD71"/>
+    <row r="71" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ71"/>
     </row>
-    <row r="72" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD72"/>
+    <row r="72" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ72"/>
     </row>
-    <row r="73" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD73"/>
+    <row r="73" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ73"/>
     </row>
-    <row r="74" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD74"/>
+    <row r="74" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ74"/>
     </row>
-    <row r="75" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD75"/>
+    <row r="75" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ75"/>
     </row>
-    <row r="76" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD76"/>
+    <row r="76" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ76"/>
     </row>
-    <row r="77" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD77"/>
+    <row r="77" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ77"/>
     </row>
-    <row r="78" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD78"/>
+    <row r="78" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ78"/>
     </row>
-    <row r="79" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD79"/>
+    <row r="79" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ79"/>
     </row>
-    <row r="80" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD80"/>
+    <row r="80" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ80"/>
     </row>
-    <row r="81" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD81"/>
+    <row r="81" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ81"/>
     </row>
-    <row r="82" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD82"/>
+    <row r="82" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ82"/>
     </row>
-    <row r="83" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD83"/>
+    <row r="83" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ83"/>
     </row>
-    <row r="84" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD84"/>
+    <row r="84" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ84"/>
     </row>
-    <row r="85" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD85"/>
+    <row r="85" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ85"/>
     </row>
-    <row r="86" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD86"/>
+    <row r="86" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ86"/>
     </row>
-    <row r="87" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD87"/>
+    <row r="87" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ87"/>
     </row>
-    <row r="88" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD88"/>
+    <row r="88" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ88"/>
     </row>
-    <row r="89" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD89"/>
+    <row r="89" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ89"/>
     </row>
-    <row r="90" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD90"/>
+    <row r="90" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ90"/>
     </row>
-    <row r="91" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD91"/>
+    <row r="91" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ91"/>
     </row>
-    <row r="92" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD92"/>
+    <row r="92" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ92"/>
     </row>
-    <row r="93" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD93"/>
+    <row r="93" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ93"/>
     </row>
-    <row r="94" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD94"/>
+    <row r="94" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ94"/>
     </row>
-    <row r="95" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD95"/>
+    <row r="95" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ95"/>
     </row>
-    <row r="96" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD96"/>
+    <row r="96" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ96"/>
     </row>
-    <row r="97" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD97"/>
+    <row r="97" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ97"/>
     </row>
-    <row r="98" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD98"/>
+    <row r="98" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ98"/>
     </row>
-    <row r="99" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD99"/>
+    <row r="99" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ99"/>
     </row>
-    <row r="100" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD100"/>
+    <row r="100" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ100"/>
     </row>
-    <row r="101" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD101"/>
+    <row r="101" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ101"/>
     </row>
-    <row r="102" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD102"/>
+    <row r="102" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ102"/>
     </row>
-    <row r="103" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD103"/>
+    <row r="103" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ103"/>
     </row>
-    <row r="104" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD104"/>
+    <row r="104" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ104"/>
     </row>
-    <row r="105" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD105"/>
+    <row r="105" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ105"/>
     </row>
-    <row r="106" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD106"/>
+    <row r="106" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ106"/>
     </row>
-    <row r="107" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD107"/>
+    <row r="107" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ107"/>
     </row>
-    <row r="108" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD108"/>
+    <row r="108" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ108"/>
     </row>
-    <row r="109" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD109"/>
+    <row r="109" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ109"/>
     </row>
-    <row r="110" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD110"/>
+    <row r="110" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ110"/>
     </row>
-    <row r="111" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD111"/>
+    <row r="111" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ111"/>
     </row>
-    <row r="112" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD112"/>
+    <row r="112" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ112"/>
     </row>
-    <row r="113" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD113"/>
+    <row r="113" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ113"/>
     </row>
-    <row r="114" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD114"/>
+    <row r="114" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ114"/>
     </row>
-    <row r="115" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD115"/>
+    <row r="115" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ115"/>
     </row>
-    <row r="116" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD116"/>
+    <row r="116" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ116"/>
     </row>
-    <row r="117" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD117"/>
+    <row r="117" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ117"/>
     </row>
-    <row r="118" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD118"/>
+    <row r="118" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ118"/>
     </row>
-    <row r="119" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD119"/>
+    <row r="119" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ119"/>
     </row>
-    <row r="120" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD120"/>
+    <row r="120" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ120"/>
     </row>
-    <row r="121" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD121"/>
+    <row r="121" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ121"/>
     </row>
-    <row r="122" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD122"/>
+    <row r="122" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ122"/>
     </row>
-    <row r="123" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD123"/>
+    <row r="123" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ123"/>
     </row>
-    <row r="124" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD124"/>
+    <row r="124" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ124"/>
     </row>
-    <row r="125" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD125"/>
+    <row r="125" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ125"/>
     </row>
-    <row r="126" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD126"/>
+    <row r="126" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ126"/>
     </row>
-    <row r="127" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD127"/>
+    <row r="127" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ127"/>
     </row>
-    <row r="128" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD128"/>
+    <row r="128" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ128"/>
     </row>
-    <row r="129" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD129"/>
+    <row r="129" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ129"/>
     </row>
-    <row r="130" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD130"/>
+    <row r="130" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ130"/>
     </row>
-    <row r="131" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD131"/>
+    <row r="131" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ131"/>
     </row>
-    <row r="132" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD132"/>
+    <row r="132" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ132"/>
     </row>
-    <row r="133" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD133"/>
+    <row r="133" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ133"/>
     </row>
-    <row r="134" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD134"/>
+    <row r="134" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ134"/>
     </row>
-    <row r="135" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD135"/>
+    <row r="135" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ135"/>
     </row>
-    <row r="136" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD136"/>
+    <row r="136" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ136"/>
     </row>
-    <row r="137" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD137"/>
+    <row r="137" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ137"/>
     </row>
-    <row r="138" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD138"/>
+    <row r="138" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ138"/>
     </row>
-    <row r="139" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD139"/>
+    <row r="139" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ139"/>
     </row>
-    <row r="140" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD140"/>
+    <row r="140" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ140"/>
     </row>
-    <row r="141" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD141"/>
+    <row r="141" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ141"/>
     </row>
-    <row r="142" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD142"/>
+    <row r="142" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ142"/>
     </row>
-    <row r="143" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD143"/>
+    <row r="143" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ143"/>
     </row>
-    <row r="144" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD144"/>
+    <row r="144" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ144"/>
     </row>
-    <row r="145" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD145"/>
+    <row r="145" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ145"/>
     </row>
-    <row r="146" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD146"/>
+    <row r="146" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ146"/>
     </row>
-    <row r="147" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD147"/>
+    <row r="147" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ147"/>
     </row>
-    <row r="148" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD148"/>
+    <row r="148" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ148"/>
     </row>
-    <row r="149" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD149"/>
+    <row r="149" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ149"/>
     </row>
-    <row r="150" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD150"/>
+    <row r="150" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ150"/>
     </row>
-    <row r="151" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD151"/>
+    <row r="151" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ151"/>
     </row>
-    <row r="152" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD152"/>
+    <row r="152" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ152"/>
     </row>
-    <row r="153" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD153"/>
+    <row r="153" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ153"/>
     </row>
-    <row r="154" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD154"/>
+    <row r="154" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ154"/>
     </row>
-    <row r="155" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD155"/>
+    <row r="155" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ155"/>
     </row>
-    <row r="156" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD156"/>
+    <row r="156" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ156"/>
     </row>
-    <row r="157" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD157"/>
+    <row r="157" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ157"/>
     </row>
-    <row r="158" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD158"/>
+    <row r="158" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ158"/>
     </row>
-    <row r="159" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD159"/>
+    <row r="159" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ159"/>
     </row>
-    <row r="160" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD160"/>
+    <row r="160" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ160"/>
     </row>
-    <row r="161" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD161"/>
+    <row r="161" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ161"/>
     </row>
-    <row r="162" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD162"/>
+    <row r="162" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ162"/>
     </row>
-    <row r="163" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD163"/>
+    <row r="163" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ163"/>
     </row>
-    <row r="164" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD164"/>
+    <row r="164" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ164"/>
     </row>
-    <row r="165" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD165"/>
+    <row r="165" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ165"/>
     </row>
-    <row r="166" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD166"/>
+    <row r="166" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ166"/>
     </row>
-    <row r="167" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD167"/>
+    <row r="167" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ167"/>
     </row>
-    <row r="168" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD168"/>
+    <row r="168" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ168"/>
     </row>
-    <row r="169" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD169"/>
+    <row r="169" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ169"/>
     </row>
-    <row r="170" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD170"/>
+    <row r="170" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ170"/>
     </row>
-    <row r="171" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD171"/>
+    <row r="171" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ171"/>
     </row>
-    <row r="172" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD172"/>
+    <row r="172" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ172"/>
     </row>
-    <row r="173" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD173"/>
+    <row r="173" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ173"/>
     </row>
-    <row r="174" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD174"/>
+    <row r="174" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ174"/>
     </row>
-    <row r="175" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD175"/>
+    <row r="175" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ175"/>
     </row>
-    <row r="176" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD176"/>
+    <row r="176" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ176"/>
     </row>
-    <row r="177" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD177"/>
+    <row r="177" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ177"/>
     </row>
-    <row r="178" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD178"/>
+    <row r="178" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ178"/>
     </row>
-    <row r="179" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD179"/>
+    <row r="179" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ179"/>
     </row>
-    <row r="180" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD180"/>
+    <row r="180" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ180"/>
     </row>
-    <row r="181" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD181"/>
+    <row r="181" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ181"/>
     </row>
-    <row r="182" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD182"/>
+    <row r="182" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ182"/>
     </row>
-    <row r="183" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD183"/>
+    <row r="183" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ183"/>
     </row>
-    <row r="184" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD184"/>
+    <row r="184" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ184"/>
     </row>
-    <row r="185" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD185"/>
+    <row r="185" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ185"/>
     </row>
-    <row r="186" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD186"/>
+    <row r="186" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ186"/>
     </row>
-    <row r="187" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD187"/>
+    <row r="187" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ187"/>
     </row>
-    <row r="188" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD188"/>
+    <row r="188" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ188"/>
     </row>
-    <row r="189" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD189"/>
+    <row r="189" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ189"/>
     </row>
-    <row r="190" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD190"/>
+    <row r="190" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ190"/>
     </row>
-    <row r="191" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD191"/>
+    <row r="191" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ191"/>
     </row>
-    <row r="192" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD192"/>
+    <row r="192" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ192"/>
     </row>
-    <row r="193" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD193"/>
+    <row r="193" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ193"/>
     </row>
-    <row r="194" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD194"/>
+    <row r="194" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ194"/>
     </row>
-    <row r="195" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD195"/>
+    <row r="195" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ195"/>
     </row>
-    <row r="196" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD196"/>
+    <row r="196" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ196"/>
     </row>
-    <row r="197" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD197"/>
+    <row r="197" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ197"/>
     </row>
-    <row r="198" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD198"/>
+    <row r="198" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ198"/>
     </row>
-    <row r="199" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD199"/>
+    <row r="199" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ199"/>
     </row>
-    <row r="200" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD200"/>
+    <row r="200" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ200"/>
     </row>
-    <row r="201" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD201"/>
+    <row r="201" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ201"/>
     </row>
-    <row r="202" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD202"/>
+    <row r="202" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ202"/>
     </row>
-    <row r="203" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD203"/>
+    <row r="203" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ203"/>
     </row>
-    <row r="204" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD204"/>
+    <row r="204" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ204"/>
     </row>
-    <row r="205" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD205"/>
+    <row r="205" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ205"/>
     </row>
-    <row r="206" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD206"/>
+    <row r="206" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ206"/>
     </row>
-    <row r="207" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD207"/>
+    <row r="207" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ207"/>
     </row>
-    <row r="208" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD208"/>
+    <row r="208" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ208"/>
     </row>
-    <row r="209" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD209"/>
+    <row r="209" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ209"/>
     </row>
-    <row r="210" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD210"/>
+    <row r="210" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ210"/>
     </row>
-    <row r="211" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD211"/>
+    <row r="211" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ211"/>
     </row>
-    <row r="212" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD212"/>
+    <row r="212" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ212"/>
     </row>
-    <row r="213" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD213"/>
+    <row r="213" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ213"/>
     </row>
-    <row r="214" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD214"/>
+    <row r="214" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ214"/>
     </row>
-    <row r="215" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD215"/>
+    <row r="215" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ215"/>
     </row>
-    <row r="216" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD216"/>
+    <row r="216" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ216"/>
     </row>
-    <row r="217" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD217"/>
+    <row r="217" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ217"/>
     </row>
-    <row r="218" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD218"/>
+    <row r="218" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ218"/>
     </row>
-    <row r="219" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD219"/>
+    <row r="219" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ219"/>
     </row>
-    <row r="220" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD220"/>
+    <row r="220" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ220"/>
     </row>
-    <row r="221" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD221"/>
+    <row r="221" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ221"/>
     </row>
-    <row r="222" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD222"/>
+    <row r="222" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ222"/>
     </row>
-    <row r="223" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD223"/>
+    <row r="223" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ223"/>
     </row>
-    <row r="224" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD224"/>
+    <row r="224" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ224"/>
     </row>
-    <row r="225" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD225"/>
+    <row r="225" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ225"/>
     </row>
-    <row r="226" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD226"/>
+    <row r="226" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ226"/>
     </row>
-    <row r="227" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD227"/>
+    <row r="227" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ227"/>
     </row>
-    <row r="228" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD228"/>
+    <row r="228" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ228"/>
     </row>
-    <row r="229" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD229"/>
+    <row r="229" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ229"/>
     </row>
-    <row r="230" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD230"/>
+    <row r="230" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ230"/>
     </row>
-    <row r="231" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD231"/>
+    <row r="231" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ231"/>
     </row>
-    <row r="232" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD232"/>
+    <row r="232" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ232"/>
     </row>
-    <row r="233" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD233"/>
+    <row r="233" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ233"/>
     </row>
-    <row r="234" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD234"/>
+    <row r="234" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ234"/>
     </row>
-    <row r="235" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD235"/>
+    <row r="235" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ235"/>
     </row>
-    <row r="236" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD236"/>
+    <row r="236" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ236"/>
     </row>
-    <row r="237" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD237"/>
+    <row r="237" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ237"/>
     </row>
-    <row r="238" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD238"/>
+    <row r="238" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ238"/>
     </row>
-    <row r="239" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD239"/>
+    <row r="239" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ239"/>
     </row>
-    <row r="240" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD240"/>
+    <row r="240" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ240"/>
     </row>
-    <row r="241" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD241"/>
+    <row r="241" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ241"/>
     </row>
-    <row r="242" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD242"/>
+    <row r="242" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ242"/>
     </row>
-    <row r="243" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD243"/>
+    <row r="243" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ243"/>
     </row>
-    <row r="244" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD244"/>
+    <row r="244" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ244"/>
     </row>
-    <row r="245" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD245"/>
+    <row r="245" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ245"/>
     </row>
-    <row r="246" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD246"/>
+    <row r="246" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ246"/>
     </row>
-    <row r="247" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD247"/>
+    <row r="247" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ247"/>
     </row>
-    <row r="248" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD248"/>
+    <row r="248" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ248"/>
     </row>
-    <row r="249" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD249"/>
+    <row r="249" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ249"/>
     </row>
-    <row r="250" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD250"/>
+    <row r="250" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ250"/>
     </row>
-    <row r="251" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD251"/>
+    <row r="251" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ251"/>
     </row>
-    <row r="252" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD252"/>
+    <row r="252" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ252"/>
     </row>
-    <row r="253" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD253"/>
+    <row r="253" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ253"/>
     </row>
-    <row r="254" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD254"/>
+    <row r="254" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ254"/>
     </row>
-    <row r="255" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD255"/>
+    <row r="255" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ255"/>
     </row>
-    <row r="256" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD256"/>
+    <row r="256" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ256"/>
     </row>
-    <row r="257" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD257"/>
+    <row r="257" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ257"/>
     </row>
-    <row r="258" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD258"/>
+    <row r="258" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ258"/>
     </row>
-    <row r="259" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD259"/>
+    <row r="259" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ259"/>
     </row>
-    <row r="260" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD260"/>
+    <row r="260" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ260"/>
     </row>
-    <row r="261" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD261"/>
+    <row r="261" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ261"/>
     </row>
-    <row r="262" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD262"/>
+    <row r="262" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ262"/>
     </row>
-    <row r="263" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD263"/>
+    <row r="263" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ263"/>
     </row>
-    <row r="264" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD264"/>
+    <row r="264" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ264"/>
     </row>
-    <row r="265" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD265"/>
+    <row r="265" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ265"/>
     </row>
-    <row r="266" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD266"/>
+    <row r="266" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ266"/>
     </row>
-    <row r="267" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD267"/>
+    <row r="267" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ267"/>
     </row>
-    <row r="268" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD268"/>
+    <row r="268" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ268"/>
     </row>
-    <row r="269" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD269"/>
+    <row r="269" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ269"/>
     </row>
-    <row r="270" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD270"/>
+    <row r="270" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ270"/>
     </row>
-    <row r="271" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD271"/>
+    <row r="271" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ271"/>
     </row>
-    <row r="272" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD272"/>
+    <row r="272" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ272"/>
     </row>
-    <row r="273" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD273"/>
+    <row r="273" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ273"/>
     </row>
-    <row r="274" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD274"/>
+    <row r="274" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ274"/>
     </row>
-    <row r="275" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD275"/>
+    <row r="275" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ275"/>
     </row>
-    <row r="276" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD276"/>
+    <row r="276" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ276"/>
     </row>
-    <row r="277" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD277"/>
+    <row r="277" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ277"/>
     </row>
-    <row r="278" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD278"/>
+    <row r="278" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ278"/>
     </row>
-    <row r="279" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD279"/>
+    <row r="279" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ279"/>
     </row>
-    <row r="280" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD280"/>
+    <row r="280" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ280"/>
     </row>
-    <row r="281" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD281"/>
+    <row r="281" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ281"/>
     </row>
-    <row r="282" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD282"/>
+    <row r="282" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ282"/>
     </row>
-    <row r="283" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD283"/>
+    <row r="283" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ283"/>
     </row>
-    <row r="284" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD284"/>
+    <row r="284" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ284"/>
     </row>
-    <row r="285" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD285"/>
+    <row r="285" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ285"/>
     </row>
-    <row r="286" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD286"/>
+    <row r="286" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ286"/>
     </row>
-    <row r="287" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD287"/>
+    <row r="287" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ287"/>
     </row>
-    <row r="288" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD288"/>
+    <row r="288" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ288"/>
     </row>
-    <row r="289" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD289"/>
+    <row r="289" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ289"/>
     </row>
-    <row r="290" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD290"/>
+    <row r="290" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ290"/>
     </row>
-    <row r="291" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD291"/>
+    <row r="291" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ291"/>
     </row>
-    <row r="292" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD292"/>
+    <row r="292" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ292"/>
     </row>
-    <row r="293" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD293"/>
+    <row r="293" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ293"/>
     </row>
-    <row r="294" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD294"/>
+    <row r="294" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ294"/>
     </row>
-    <row r="295" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD295"/>
+    <row r="295" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ295"/>
     </row>
-    <row r="296" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD296"/>
+    <row r="296" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ296"/>
     </row>
-    <row r="297" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD297"/>
+    <row r="297" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ297"/>
     </row>
-    <row r="298" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD298"/>
+    <row r="298" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ298"/>
     </row>
-    <row r="299" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD299"/>
+    <row r="299" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ299"/>
     </row>
-    <row r="300" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD300"/>
+    <row r="300" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ300"/>
     </row>
-    <row r="301" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD301"/>
+    <row r="301" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ301"/>
     </row>
-    <row r="302" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD302"/>
+    <row r="302" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ302"/>
     </row>
-    <row r="303" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD303"/>
+    <row r="303" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ303"/>
     </row>
-    <row r="304" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD304"/>
+    <row r="304" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ304"/>
     </row>
-    <row r="305" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD305"/>
+    <row r="305" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ305"/>
     </row>
-    <row r="306" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD306"/>
+    <row r="306" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ306"/>
     </row>
-    <row r="307" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD307"/>
+    <row r="307" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ307"/>
     </row>
-    <row r="308" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD308"/>
+    <row r="308" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ308"/>
     </row>
-    <row r="309" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD309"/>
+    <row r="309" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ309"/>
     </row>
-    <row r="310" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD310"/>
+    <row r="310" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ310"/>
     </row>
-    <row r="311" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD311"/>
+    <row r="311" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ311"/>
     </row>
-    <row r="312" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD312"/>
+    <row r="312" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ312"/>
     </row>
-    <row r="313" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD313"/>
+    <row r="313" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ313"/>
     </row>
-    <row r="314" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD314"/>
+    <row r="314" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ314"/>
     </row>
-    <row r="315" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD315"/>
+    <row r="315" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ315"/>
     </row>
-    <row r="316" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD316"/>
+    <row r="316" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ316"/>
     </row>
-    <row r="317" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD317"/>
+    <row r="317" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ317"/>
     </row>
-    <row r="318" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD318"/>
+    <row r="318" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ318"/>
     </row>
-    <row r="319" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD319"/>
+    <row r="319" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ319"/>
     </row>
-    <row r="320" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD320"/>
+    <row r="320" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ320"/>
     </row>
-    <row r="321" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD321"/>
+    <row r="321" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ321"/>
     </row>
-    <row r="322" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD322"/>
+    <row r="322" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ322"/>
     </row>
-    <row r="323" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD323"/>
+    <row r="323" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ323"/>
     </row>
-    <row r="324" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD324"/>
+    <row r="324" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ324"/>
     </row>
-    <row r="325" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD325"/>
+    <row r="325" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ325"/>
     </row>
-    <row r="326" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD326"/>
+    <row r="326" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ326"/>
     </row>
-    <row r="327" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD327"/>
+    <row r="327" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ327"/>
     </row>
-    <row r="328" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD328"/>
+    <row r="328" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ328"/>
     </row>
-    <row r="329" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD329"/>
+    <row r="329" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ329"/>
     </row>
-    <row r="330" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD330"/>
+    <row r="330" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ330"/>
     </row>
-    <row r="331" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD331"/>
+    <row r="331" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ331"/>
     </row>
-    <row r="332" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD332"/>
+    <row r="332" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ332"/>
     </row>
-    <row r="333" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD333"/>
+    <row r="333" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ333"/>
     </row>
-    <row r="334" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD334"/>
+    <row r="334" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ334"/>
     </row>
-    <row r="335" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD335"/>
+    <row r="335" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ335"/>
     </row>
-    <row r="336" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD336"/>
+    <row r="336" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ336"/>
     </row>
-    <row r="337" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD337"/>
+    <row r="337" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ337"/>
     </row>
-    <row r="338" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD338"/>
+    <row r="338" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ338"/>
     </row>
-    <row r="339" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD339"/>
+    <row r="339" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ339"/>
     </row>
-    <row r="340" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD340"/>
+    <row r="340" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ340"/>
     </row>
-    <row r="341" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD341"/>
+    <row r="341" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ341"/>
     </row>
-    <row r="342" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD342"/>
+    <row r="342" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ342"/>
     </row>
-    <row r="343" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD343"/>
+    <row r="343" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ343"/>
     </row>
-    <row r="344" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD344"/>
+    <row r="344" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ344"/>
     </row>
-    <row r="345" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD345"/>
+    <row r="345" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ345"/>
     </row>
-    <row r="346" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD346"/>
+    <row r="346" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ346"/>
     </row>
-    <row r="347" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD347"/>
+    <row r="347" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ347"/>
     </row>
-    <row r="348" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD348"/>
+    <row r="348" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ348"/>
     </row>
-    <row r="349" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD349"/>
+    <row r="349" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ349"/>
     </row>
-    <row r="350" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD350"/>
+    <row r="350" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ350"/>
     </row>
-    <row r="351" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD351"/>
+    <row r="351" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ351"/>
     </row>
-    <row r="352" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD352"/>
+    <row r="352" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ352"/>
     </row>
-    <row r="353" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD353"/>
+    <row r="353" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ353"/>
     </row>
-    <row r="354" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD354"/>
+    <row r="354" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ354"/>
     </row>
-    <row r="355" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD355"/>
+    <row r="355" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ355"/>
     </row>
-    <row r="356" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD356"/>
+    <row r="356" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ356"/>
     </row>
-    <row r="357" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD357"/>
+    <row r="357" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ357"/>
     </row>
-    <row r="358" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD358"/>
+    <row r="358" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ358"/>
     </row>
-    <row r="359" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD359"/>
+    <row r="359" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ359"/>
     </row>
-    <row r="360" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD360"/>
+    <row r="360" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ360"/>
     </row>
-    <row r="361" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD361"/>
+    <row r="361" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ361"/>
     </row>
-    <row r="362" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD362"/>
+    <row r="362" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ362"/>
     </row>
-    <row r="363" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD363"/>
+    <row r="363" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ363"/>
     </row>
-    <row r="364" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD364"/>
+    <row r="364" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ364"/>
     </row>
-    <row r="365" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD365"/>
+    <row r="365" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ365"/>
     </row>
-    <row r="366" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD366"/>
+    <row r="366" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ366"/>
     </row>
-    <row r="367" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD367"/>
+    <row r="367" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ367"/>
     </row>
-    <row r="368" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD368"/>
+    <row r="368" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ368"/>
     </row>
-    <row r="369" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD369"/>
+    <row r="369" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ369"/>
     </row>
-    <row r="370" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD370"/>
+    <row r="370" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ370"/>
     </row>
-    <row r="371" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD371"/>
+    <row r="371" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ371"/>
     </row>
-    <row r="372" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD372"/>
+    <row r="372" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ372"/>
     </row>
-    <row r="373" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD373"/>
+    <row r="373" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ373"/>
     </row>
-    <row r="374" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD374"/>
+    <row r="374" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ374"/>
     </row>
-    <row r="375" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD375"/>
+    <row r="375" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ375"/>
     </row>
-    <row r="376" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD376"/>
+    <row r="376" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ376"/>
     </row>
-    <row r="377" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD377"/>
+    <row r="377" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ377"/>
     </row>
-    <row r="378" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD378"/>
+    <row r="378" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ378"/>
     </row>
-    <row r="379" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD379"/>
+    <row r="379" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ379"/>
     </row>
-    <row r="380" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD380"/>
+    <row r="380" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ380"/>
     </row>
-    <row r="381" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD381"/>
+    <row r="381" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ381"/>
     </row>
-    <row r="382" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD382"/>
+    <row r="382" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ382"/>
     </row>
-    <row r="383" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD383"/>
+    <row r="383" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ383"/>
     </row>
-    <row r="384" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD384"/>
+    <row r="384" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ384"/>
     </row>
-    <row r="385" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD385"/>
+    <row r="385" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ385"/>
     </row>
-    <row r="386" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD386"/>
+    <row r="386" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ386"/>
     </row>
-    <row r="387" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD387"/>
+    <row r="387" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ387"/>
     </row>
-    <row r="388" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD388"/>
+    <row r="388" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ388"/>
     </row>
-    <row r="389" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD389"/>
+    <row r="389" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ389"/>
     </row>
-    <row r="390" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD390"/>
+    <row r="390" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ390"/>
     </row>
-    <row r="391" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD391"/>
+    <row r="391" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ391"/>
     </row>
-    <row r="392" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD392"/>
+    <row r="392" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ392"/>
     </row>
-    <row r="393" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD393"/>
+    <row r="393" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ393"/>
     </row>
-    <row r="394" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD394"/>
+    <row r="394" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ394"/>
     </row>
-    <row r="395" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD395"/>
+    <row r="395" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ395"/>
     </row>
-    <row r="396" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD396"/>
+    <row r="396" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ396"/>
     </row>
-    <row r="397" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD397"/>
+    <row r="397" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ397"/>
     </row>
-    <row r="398" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD398"/>
+    <row r="398" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ398"/>
     </row>
-    <row r="399" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD399"/>
+    <row r="399" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ399"/>
     </row>
-    <row r="400" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD400"/>
+    <row r="400" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ400"/>
     </row>
-    <row r="401" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD401"/>
+    <row r="401" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ401"/>
     </row>
-    <row r="402" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD402"/>
+    <row r="402" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ402"/>
     </row>
-    <row r="403" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD403"/>
+    <row r="403" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ403"/>
     </row>
-    <row r="404" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD404"/>
+    <row r="404" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ404"/>
     </row>
-    <row r="405" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD405"/>
+    <row r="405" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ405"/>
     </row>
-    <row r="406" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD406"/>
+    <row r="406" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ406"/>
     </row>
-    <row r="407" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD407"/>
+    <row r="407" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ407"/>
     </row>
-    <row r="408" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD408"/>
+    <row r="408" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ408"/>
     </row>
-    <row r="409" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD409"/>
+    <row r="409" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ409"/>
     </row>
-    <row r="410" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD410"/>
+    <row r="410" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ410"/>
     </row>
-    <row r="411" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD411"/>
+    <row r="411" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ411"/>
     </row>
-    <row r="412" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD412"/>
+    <row r="412" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ412"/>
     </row>
-    <row r="413" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD413"/>
+    <row r="413" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ413"/>
     </row>
-    <row r="414" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD414"/>
+    <row r="414" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ414"/>
     </row>
-    <row r="415" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD415"/>
+    <row r="415" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ415"/>
     </row>
-    <row r="416" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD416"/>
+    <row r="416" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ416"/>
     </row>
-    <row r="417" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD417"/>
+    <row r="417" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ417"/>
     </row>
-    <row r="418" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD418"/>
+    <row r="418" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ418"/>
     </row>
-    <row r="419" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD419"/>
+    <row r="419" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ419"/>
     </row>
-    <row r="420" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD420"/>
+    <row r="420" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ420"/>
     </row>
-    <row r="421" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD421"/>
+    <row r="421" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ421"/>
     </row>
-    <row r="422" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD422"/>
+    <row r="422" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ422"/>
     </row>
-    <row r="423" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD423"/>
+    <row r="423" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ423"/>
     </row>
-    <row r="424" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD424"/>
+    <row r="424" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ424"/>
     </row>
-    <row r="425" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD425"/>
+    <row r="425" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ425"/>
     </row>
-    <row r="426" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD426"/>
+    <row r="426" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ426"/>
     </row>
-    <row r="427" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD427"/>
+    <row r="427" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ427"/>
     </row>
-    <row r="428" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD428"/>
+    <row r="428" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ428"/>
     </row>
-    <row r="429" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD429"/>
+    <row r="429" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ429"/>
     </row>
-    <row r="430" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD430"/>
+    <row r="430" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ430"/>
     </row>
-    <row r="431" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD431"/>
+    <row r="431" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ431"/>
     </row>
-    <row r="432" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD432"/>
+    <row r="432" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ432"/>
     </row>
-    <row r="433" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD433"/>
+    <row r="433" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ433"/>
     </row>
-    <row r="434" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD434"/>
+    <row r="434" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ434"/>
     </row>
-    <row r="435" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD435"/>
+    <row r="435" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ435"/>
     </row>
-    <row r="436" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD436"/>
+    <row r="436" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ436"/>
     </row>
-    <row r="437" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD437"/>
+    <row r="437" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ437"/>
     </row>
-    <row r="438" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD438"/>
+    <row r="438" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ438"/>
     </row>
-    <row r="439" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD439"/>
+    <row r="439" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ439"/>
     </row>
-    <row r="440" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD440"/>
+    <row r="440" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ440"/>
     </row>
-    <row r="441" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD441"/>
+    <row r="441" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ441"/>
     </row>
-    <row r="442" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD442"/>
+    <row r="442" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ442"/>
     </row>
-    <row r="443" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD443"/>
+    <row r="443" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ443"/>
     </row>
-    <row r="444" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD444"/>
+    <row r="444" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ444"/>
     </row>
-    <row r="445" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD445"/>
+    <row r="445" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ445"/>
     </row>
-    <row r="446" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD446"/>
+    <row r="446" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ446"/>
     </row>
-    <row r="447" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD447"/>
+    <row r="447" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ447"/>
     </row>
-    <row r="448" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD448"/>
+    <row r="448" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ448"/>
     </row>
-    <row r="449" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD449"/>
+    <row r="449" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ449"/>
     </row>
-    <row r="450" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD450"/>
+    <row r="450" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ450"/>
     </row>
-    <row r="451" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD451"/>
+    <row r="451" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ451"/>
     </row>
-    <row r="452" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD452"/>
+    <row r="452" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ452"/>
     </row>
-    <row r="453" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD453"/>
+    <row r="453" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ453"/>
     </row>
-    <row r="454" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD454"/>
+    <row r="454" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ454"/>
     </row>
-    <row r="455" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD455"/>
+    <row r="455" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ455"/>
     </row>
-    <row r="456" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD456"/>
+    <row r="456" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ456"/>
     </row>
-    <row r="457" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD457"/>
+    <row r="457" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ457"/>
     </row>
-    <row r="458" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD458"/>
+    <row r="458" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ458"/>
     </row>
-    <row r="459" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD459"/>
+    <row r="459" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ459"/>
     </row>
-    <row r="460" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD460"/>
+    <row r="460" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ460"/>
     </row>
-    <row r="461" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD461"/>
+    <row r="461" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ461"/>
     </row>
-    <row r="462" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD462"/>
+    <row r="462" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ462"/>
     </row>
-    <row r="463" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD463"/>
+    <row r="463" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ463"/>
     </row>
-    <row r="464" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD464"/>
+    <row r="464" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ464"/>
     </row>
-    <row r="465" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD465"/>
+    <row r="465" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ465"/>
     </row>
-    <row r="466" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD466"/>
+    <row r="466" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ466"/>
     </row>
-    <row r="467" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD467"/>
+    <row r="467" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ467"/>
     </row>
-    <row r="468" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD468"/>
+    <row r="468" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ468"/>
     </row>
-    <row r="469" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD469"/>
+    <row r="469" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ469"/>
     </row>
-    <row r="470" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD470"/>
+    <row r="470" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ470"/>
     </row>
-    <row r="471" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD471"/>
+    <row r="471" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ471"/>
     </row>
-    <row r="472" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD472"/>
+    <row r="472" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ472"/>
     </row>
-    <row r="473" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD473"/>
+    <row r="473" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ473"/>
     </row>
-    <row r="474" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD474"/>
+    <row r="474" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ474"/>
     </row>
-    <row r="475" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD475"/>
+    <row r="475" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ475"/>
     </row>
-    <row r="476" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD476"/>
+    <row r="476" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ476"/>
     </row>
-    <row r="477" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD477"/>
+    <row r="477" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ477"/>
     </row>
-    <row r="478" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD478"/>
+    <row r="478" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ478"/>
     </row>
-    <row r="479" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD479"/>
+    <row r="479" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ479"/>
     </row>
-    <row r="480" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD480"/>
+    <row r="480" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ480"/>
     </row>
-    <row r="481" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD481"/>
+    <row r="481" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ481"/>
     </row>
-    <row r="482" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD482"/>
+    <row r="482" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ482"/>
     </row>
-    <row r="483" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD483"/>
+    <row r="483" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ483"/>
     </row>
-    <row r="484" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD484"/>
+    <row r="484" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ484"/>
     </row>
-    <row r="485" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD485"/>
+    <row r="485" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ485"/>
     </row>
-    <row r="486" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD486"/>
+    <row r="486" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ486"/>
     </row>
-    <row r="487" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD487"/>
+    <row r="487" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ487"/>
     </row>
-    <row r="488" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD488"/>
+    <row r="488" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ488"/>
     </row>
-    <row r="489" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD489"/>
+    <row r="489" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ489"/>
     </row>
-    <row r="490" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD490"/>
+    <row r="490" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ490"/>
     </row>
-    <row r="491" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD491"/>
+    <row r="491" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ491"/>
     </row>
-    <row r="492" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD492"/>
+    <row r="492" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ492"/>
     </row>
-    <row r="493" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD493"/>
+    <row r="493" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ493"/>
     </row>
-    <row r="494" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD494"/>
+    <row r="494" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ494"/>
     </row>
-    <row r="495" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD495"/>
+    <row r="495" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ495"/>
     </row>
-    <row r="496" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD496"/>
+    <row r="496" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ496"/>
     </row>
-    <row r="497" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD497"/>
+    <row r="497" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ497"/>
     </row>
-    <row r="498" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD498"/>
+    <row r="498" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ498"/>
     </row>
-    <row r="499" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD499"/>
+    <row r="499" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ499"/>
     </row>
-    <row r="500" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD500"/>
+    <row r="500" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ500"/>
     </row>
-    <row r="501" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD501"/>
+    <row r="501" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ501"/>
     </row>
-    <row r="502" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD502"/>
+    <row r="502" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ502"/>
     </row>
-    <row r="503" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD503"/>
+    <row r="503" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ503"/>
     </row>
-    <row r="504" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD504"/>
+    <row r="504" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ504"/>
     </row>
-    <row r="505" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD505"/>
+    <row r="505" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ505"/>
     </row>
-    <row r="506" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD506"/>
+    <row r="506" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ506"/>
     </row>
-    <row r="507" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD507"/>
+    <row r="507" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ507"/>
     </row>
-    <row r="508" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD508"/>
+    <row r="508" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ508"/>
     </row>
-    <row r="509" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD509"/>
+    <row r="509" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ509"/>
     </row>
-    <row r="510" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD510"/>
+    <row r="510" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ510"/>
     </row>
-    <row r="511" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD511"/>
+    <row r="511" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ511"/>
     </row>
-    <row r="512" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD512"/>
+    <row r="512" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ512"/>
     </row>
-    <row r="513" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD513"/>
+    <row r="513" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ513"/>
     </row>
-    <row r="514" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD514"/>
+    <row r="514" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ514"/>
     </row>
-    <row r="515" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD515"/>
+    <row r="515" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ515"/>
     </row>
-    <row r="516" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD516"/>
+    <row r="516" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ516"/>
     </row>
-    <row r="517" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD517"/>
+    <row r="517" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ517"/>
     </row>
-    <row r="518" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD518"/>
+    <row r="518" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ518"/>
     </row>
-    <row r="519" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD519"/>
+    <row r="519" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ519"/>
     </row>
-    <row r="520" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD520"/>
+    <row r="520" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ520"/>
     </row>
-    <row r="521" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD521"/>
+    <row r="521" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ521"/>
     </row>
-    <row r="522" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD522"/>
+    <row r="522" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ522"/>
     </row>
-    <row r="523" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD523"/>
+    <row r="523" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ523"/>
     </row>
-    <row r="524" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD524"/>
+    <row r="524" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ524"/>
     </row>
-    <row r="525" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD525"/>
+    <row r="525" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ525"/>
     </row>
-    <row r="526" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD526"/>
+    <row r="526" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ526"/>
     </row>
-    <row r="527" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD527"/>
+    <row r="527" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ527"/>
     </row>
-    <row r="528" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD528"/>
+    <row r="528" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ528"/>
     </row>
-    <row r="529" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD529"/>
+    <row r="529" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ529"/>
     </row>
-    <row r="530" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD530"/>
+    <row r="530" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ530"/>
     </row>
-    <row r="531" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD531"/>
+    <row r="531" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ531"/>
     </row>
-    <row r="532" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD532"/>
+    <row r="532" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ532"/>
     </row>
-    <row r="533" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD533"/>
+    <row r="533" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ533"/>
     </row>
-    <row r="534" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD534"/>
+    <row r="534" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ534"/>
     </row>
-    <row r="535" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD535"/>
+    <row r="535" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ535"/>
     </row>
-    <row r="536" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD536"/>
+    <row r="536" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ536"/>
     </row>
-    <row r="537" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD537"/>
+    <row r="537" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ537"/>
     </row>
-    <row r="538" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD538"/>
+    <row r="538" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ538"/>
     </row>
-    <row r="539" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD539"/>
+    <row r="539" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ539"/>
     </row>
-    <row r="540" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD540"/>
+    <row r="540" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ540"/>
     </row>
-    <row r="541" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD541"/>
+    <row r="541" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ541"/>
     </row>
-    <row r="542" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD542"/>
+    <row r="542" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ542"/>
     </row>
-    <row r="543" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD543"/>
+    <row r="543" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ543"/>
     </row>
-    <row r="544" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD544"/>
+    <row r="544" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ544"/>
     </row>
-    <row r="545" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD545"/>
+    <row r="545" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ545"/>
     </row>
-    <row r="546" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD546"/>
+    <row r="546" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ546"/>
     </row>
-    <row r="547" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD547"/>
+    <row r="547" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ547"/>
     </row>
-    <row r="548" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD548"/>
+    <row r="548" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ548"/>
     </row>
-    <row r="549" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD549"/>
+    <row r="549" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ549"/>
     </row>
-    <row r="550" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD550"/>
+    <row r="550" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ550"/>
     </row>
-    <row r="551" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD551"/>
+    <row r="551" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ551"/>
     </row>
-    <row r="552" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD552"/>
+    <row r="552" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ552"/>
     </row>
-    <row r="553" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD553"/>
+    <row r="553" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ553"/>
     </row>
-    <row r="554" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD554"/>
+    <row r="554" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ554"/>
     </row>
-    <row r="555" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD555"/>
+    <row r="555" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ555"/>
     </row>
-    <row r="556" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD556"/>
+    <row r="556" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ556"/>
     </row>
-    <row r="557" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD557"/>
+    <row r="557" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ557"/>
     </row>
-    <row r="558" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD558"/>
+    <row r="558" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ558"/>
     </row>
-    <row r="559" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD559"/>
+    <row r="559" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ559"/>
     </row>
-    <row r="560" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD560"/>
+    <row r="560" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ560"/>
     </row>
-    <row r="561" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD561"/>
+    <row r="561" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ561"/>
     </row>
-    <row r="562" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD562"/>
+    <row r="562" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ562"/>
     </row>
-    <row r="563" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD563"/>
+    <row r="563" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ563"/>
     </row>
-    <row r="564" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD564"/>
+    <row r="564" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ564"/>
     </row>
-    <row r="565" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD565"/>
+    <row r="565" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ565"/>
     </row>
-    <row r="566" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD566"/>
+    <row r="566" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ566"/>
     </row>
-    <row r="567" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD567"/>
+    <row r="567" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ567"/>
     </row>
-    <row r="568" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD568"/>
+    <row r="568" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ568"/>
     </row>
-    <row r="569" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD569"/>
+    <row r="569" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ569"/>
     </row>
-    <row r="570" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD570"/>
+    <row r="570" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ570"/>
     </row>
-    <row r="571" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD571"/>
+    <row r="571" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ571"/>
     </row>
-    <row r="572" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD572"/>
+    <row r="572" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ572"/>
     </row>
-    <row r="573" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD573"/>
+    <row r="573" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ573"/>
     </row>
-    <row r="574" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD574"/>
+    <row r="574" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ574"/>
     </row>
-    <row r="575" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD575"/>
+    <row r="575" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ575"/>
     </row>
-    <row r="576" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD576"/>
+    <row r="576" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ576"/>
     </row>
-    <row r="577" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD577"/>
+    <row r="577" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ577"/>
     </row>
-    <row r="578" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD578"/>
+    <row r="578" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ578"/>
     </row>
-    <row r="579" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD579"/>
+    <row r="579" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ579"/>
     </row>
-    <row r="580" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD580"/>
+    <row r="580" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ580"/>
     </row>
-    <row r="581" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD581"/>
+    <row r="581" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ581"/>
     </row>
-    <row r="582" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD582"/>
+    <row r="582" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ582"/>
     </row>
-    <row r="583" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD583"/>
+    <row r="583" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ583"/>
     </row>
-    <row r="584" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD584"/>
+    <row r="584" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ584"/>
     </row>
-    <row r="585" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD585"/>
+    <row r="585" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ585"/>
     </row>
-    <row r="586" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD586"/>
+    <row r="586" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ586"/>
     </row>
-    <row r="587" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD587"/>
+    <row r="587" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ587"/>
     </row>
-    <row r="588" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD588"/>
+    <row r="588" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ588"/>
     </row>
-    <row r="589" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD589"/>
+    <row r="589" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ589"/>
     </row>
-    <row r="590" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD590"/>
+    <row r="590" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ590"/>
     </row>
-    <row r="591" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD591"/>
+    <row r="591" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ591"/>
     </row>
-    <row r="592" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD592"/>
+    <row r="592" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ592"/>
     </row>
-    <row r="593" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD593"/>
+    <row r="593" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ593"/>
     </row>
-    <row r="594" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD594"/>
+    <row r="594" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ594"/>
     </row>
-    <row r="595" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD595"/>
+    <row r="595" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ595"/>
     </row>
-    <row r="596" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD596"/>
+    <row r="596" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ596"/>
     </row>
-    <row r="597" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD597"/>
+    <row r="597" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ597"/>
     </row>
-    <row r="598" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD598"/>
+    <row r="598" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ598"/>
     </row>
-    <row r="599" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD599"/>
+    <row r="599" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ599"/>
     </row>
-    <row r="600" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD600"/>
+    <row r="600" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ600"/>
     </row>
-    <row r="601" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD601"/>
+    <row r="601" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ601"/>
     </row>
-    <row r="602" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD602"/>
+    <row r="602" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ602"/>
     </row>
-    <row r="603" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD603"/>
+    <row r="603" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ603"/>
     </row>
-    <row r="604" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD604"/>
+    <row r="604" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ604"/>
     </row>
-    <row r="605" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD605"/>
+    <row r="605" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ605"/>
     </row>
-    <row r="606" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD606"/>
+    <row r="606" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ606"/>
     </row>
-    <row r="607" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD607"/>
+    <row r="607" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ607"/>
     </row>
-    <row r="608" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD608"/>
+    <row r="608" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ608"/>
     </row>
-    <row r="609" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD609"/>
+    <row r="609" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ609"/>
     </row>
-    <row r="610" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD610"/>
+    <row r="610" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ610"/>
     </row>
-    <row r="611" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD611"/>
+    <row r="611" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ611"/>
     </row>
-    <row r="612" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD612"/>
+    <row r="612" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ612"/>
     </row>
-    <row r="613" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD613"/>
+    <row r="613" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ613"/>
     </row>
-    <row r="614" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD614"/>
+    <row r="614" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ614"/>
     </row>
-    <row r="615" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD615"/>
+    <row r="615" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ615"/>
     </row>
-    <row r="616" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD616"/>
+    <row r="616" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ616"/>
     </row>
-    <row r="617" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD617"/>
+    <row r="617" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ617"/>
     </row>
-    <row r="618" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD618"/>
+    <row r="618" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ618"/>
     </row>
-    <row r="619" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD619"/>
+    <row r="619" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ619"/>
     </row>
-    <row r="620" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD620"/>
+    <row r="620" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ620"/>
     </row>
-    <row r="621" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD621"/>
+    <row r="621" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ621"/>
     </row>
-    <row r="622" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD622"/>
+    <row r="622" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ622"/>
     </row>
-    <row r="623" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD623"/>
+    <row r="623" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ623"/>
     </row>
-    <row r="624" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD624"/>
+    <row r="624" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ624"/>
     </row>
-    <row r="625" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD625"/>
+    <row r="625" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ625"/>
     </row>
-    <row r="626" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD626"/>
+    <row r="626" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ626"/>
     </row>
-    <row r="627" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD627"/>
+    <row r="627" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ627"/>
     </row>
-    <row r="628" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD628"/>
+    <row r="628" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ628"/>
     </row>
-    <row r="629" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD629"/>
+    <row r="629" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ629"/>
     </row>
-    <row r="630" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD630"/>
+    <row r="630" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ630"/>
     </row>
-    <row r="631" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD631"/>
+    <row r="631" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ631"/>
     </row>
-    <row r="632" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD632"/>
+    <row r="632" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ632"/>
     </row>
-    <row r="633" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD633"/>
+    <row r="633" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ633"/>
     </row>
-    <row r="634" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD634"/>
+    <row r="634" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ634"/>
     </row>
-    <row r="635" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD635"/>
+    <row r="635" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ635"/>
     </row>
-    <row r="636" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD636"/>
+    <row r="636" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ636"/>
     </row>
-    <row r="637" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD637"/>
+    <row r="637" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ637"/>
     </row>
-    <row r="638" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD638"/>
+    <row r="638" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ638"/>
     </row>
-    <row r="639" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD639"/>
+    <row r="639" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ639"/>
     </row>
-    <row r="640" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD640"/>
+    <row r="640" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ640"/>
     </row>
-    <row r="641" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD641"/>
+    <row r="641" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ641"/>
     </row>
-    <row r="642" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD642"/>
+    <row r="642" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ642"/>
     </row>
-    <row r="643" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD643"/>
+    <row r="643" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ643"/>
     </row>
-    <row r="644" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD644"/>
+    <row r="644" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ644"/>
     </row>
-    <row r="645" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD645"/>
+    <row r="645" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ645"/>
     </row>
-    <row r="646" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD646"/>
+    <row r="646" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ646"/>
     </row>
-    <row r="647" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD647"/>
+    <row r="647" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ647"/>
     </row>
-    <row r="648" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD648"/>
+    <row r="648" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ648"/>
     </row>
-    <row r="649" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD649"/>
+    <row r="649" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ649"/>
     </row>
-    <row r="650" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD650"/>
+    <row r="650" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ650"/>
     </row>
-    <row r="651" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD651"/>
+    <row r="651" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ651"/>
     </row>
-    <row r="652" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD652"/>
+    <row r="652" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ652"/>
     </row>
-    <row r="653" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD653"/>
+    <row r="653" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ653"/>
     </row>
-    <row r="654" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD654"/>
+    <row r="654" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ654"/>
     </row>
-    <row r="655" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD655"/>
+    <row r="655" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ655"/>
     </row>
-    <row r="656" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD656"/>
+    <row r="656" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ656"/>
     </row>
-    <row r="657" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD657"/>
+    <row r="657" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ657"/>
     </row>
-    <row r="658" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD658"/>
+    <row r="658" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ658"/>
     </row>
-    <row r="659" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD659"/>
+    <row r="659" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ659"/>
     </row>
-    <row r="660" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD660"/>
+    <row r="660" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ660"/>
     </row>
-    <row r="661" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD661"/>
+    <row r="661" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ661"/>
     </row>
-    <row r="662" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD662"/>
+    <row r="662" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ662"/>
     </row>
-    <row r="663" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD663"/>
+    <row r="663" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ663"/>
     </row>
-    <row r="664" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD664"/>
+    <row r="664" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ664"/>
     </row>
-    <row r="665" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD665"/>
+    <row r="665" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ665"/>
     </row>
-    <row r="666" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD666"/>
+    <row r="666" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ666"/>
     </row>
-    <row r="667" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD667"/>
+    <row r="667" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ667"/>
     </row>
-    <row r="668" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD668"/>
+    <row r="668" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ668"/>
     </row>
-    <row r="669" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD669"/>
+    <row r="669" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ669"/>
     </row>
-    <row r="670" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD670"/>
+    <row r="670" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ670"/>
     </row>
-    <row r="671" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD671"/>
+    <row r="671" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ671"/>
     </row>
-    <row r="672" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD672"/>
+    <row r="672" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ672"/>
     </row>
-    <row r="673" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD673"/>
+    <row r="673" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ673"/>
     </row>
-    <row r="674" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD674"/>
+    <row r="674" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ674"/>
     </row>
-    <row r="675" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD675"/>
+    <row r="675" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ675"/>
     </row>
-    <row r="676" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD676"/>
+    <row r="676" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ676"/>
     </row>
-    <row r="677" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD677"/>
+    <row r="677" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ677"/>
     </row>
-    <row r="678" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD678"/>
+    <row r="678" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ678"/>
     </row>
-    <row r="679" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD679"/>
+    <row r="679" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ679"/>
     </row>
-    <row r="680" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD680"/>
+    <row r="680" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ680"/>
     </row>
-    <row r="681" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD681"/>
+    <row r="681" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ681"/>
     </row>
-    <row r="682" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD682"/>
+    <row r="682" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ682"/>
     </row>
-    <row r="683" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD683"/>
+    <row r="683" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ683"/>
     </row>
-    <row r="684" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD684"/>
+    <row r="684" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ684"/>
     </row>
-    <row r="685" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD685"/>
+    <row r="685" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ685"/>
     </row>
-    <row r="686" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD686"/>
+    <row r="686" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ686"/>
     </row>
-    <row r="687" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD687"/>
+    <row r="687" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ687"/>
     </row>
-    <row r="688" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD688"/>
+    <row r="688" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ688"/>
     </row>
-    <row r="689" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD689"/>
+    <row r="689" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ689"/>
     </row>
-    <row r="690" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD690"/>
+    <row r="690" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ690"/>
     </row>
-    <row r="691" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD691"/>
+    <row r="691" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ691"/>
     </row>
-    <row r="692" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD692"/>
+    <row r="692" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ692"/>
     </row>
-    <row r="693" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD693"/>
+    <row r="693" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ693"/>
     </row>
-    <row r="694" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD694"/>
+    <row r="694" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ694"/>
     </row>
-    <row r="695" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD695"/>
+    <row r="695" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ695"/>
     </row>
-    <row r="696" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD696"/>
+    <row r="696" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ696"/>
     </row>
-    <row r="697" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD697"/>
+    <row r="697" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ697"/>
     </row>
-    <row r="698" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD698"/>
+    <row r="698" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ698"/>
     </row>
-    <row r="699" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD699"/>
+    <row r="699" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ699"/>
     </row>
-    <row r="700" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD700"/>
+    <row r="700" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ700"/>
     </row>
-    <row r="701" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD701"/>
+    <row r="701" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ701"/>
     </row>
-    <row r="702" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD702"/>
+    <row r="702" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ702"/>
     </row>
-    <row r="703" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD703"/>
+    <row r="703" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ703"/>
     </row>
-    <row r="704" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD704"/>
+    <row r="704" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ704"/>
     </row>
-    <row r="705" spans="56:130" x14ac:dyDescent="0.25">
-      <c r="BD705"/>
+    <row r="705" spans="130:130" x14ac:dyDescent="0.25">
       <c r="DZ705"/>
     </row>
   </sheetData>

</xml_diff>